<commit_message>
1.0.11 features and some bugfixes
</commit_message>
<xml_diff>
--- a/ASSETS/excel/ticker/ticker_facts.xlsx
+++ b/ASSETS/excel/ticker/ticker_facts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GC\ASSETS\excel\ticker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6436667-7457-465B-B749-B70D75F2A091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D1C9DA-E4D9-4949-B210-5C007B5C1BA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="2640" windowWidth="32115" windowHeight="18045" activeTab="3" xr2:uid="{D3602A80-A8D3-45A9-BF39-551D68E1E11E}"/>
+    <workbookView xWindow="16755" yWindow="6285" windowWidth="40845" windowHeight="12795" xr2:uid="{D3602A80-A8D3-45A9-BF39-551D68E1E11E}"/>
   </bookViews>
   <sheets>
     <sheet name="#README" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>TICKER ITEM TEXT</t>
   </si>
@@ -572,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5219D8A8-C5B7-4081-B580-34C8F58A105A}">
   <dimension ref="B2:B3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -604,7 +604,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,9 +643,6 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
@@ -808,7 +805,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A50">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1059,7 +1056,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A47">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1074,7 +1071,7 @@
   </sheetPr>
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1259,7 +1256,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A48">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>